<commit_message>
Update Filter Filtration Factor Testing 2020.04.20 AccuFIT AS WN with pic.xlsx
</commit_message>
<xml_diff>
--- a/04-Testing/Results/Filter Filtration Factor Testing 2020.04.20 AccuFIT AS WN with pic.xlsx
+++ b/04-Testing/Results/Filter Filtration Factor Testing 2020.04.20 AccuFIT AS WN with pic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wckng/Documents/Medicine/Research Writing/UofT 2019-2022/COVID-19/COVID Refs/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wckng/Documents/GitHub/Reusable-N95-Project/04-Testing/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18B7D21C-54C7-FC45-8275-E087C734469C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDD1FA1-75A9-AB40-83DA-E04A4915BD4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{08DD48C9-3845-9945-B0E9-9104EFD45640}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16940" xr2:uid="{08DD48C9-3845-9945-B0E9-9104EFD45640}"/>
   </bookViews>
   <sheets>
     <sheet name="Filtration Factors" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Date:</t>
   </si>
@@ -72,48 +72,18 @@
     <t>Average Filtration Factor</t>
   </si>
   <si>
-    <t>Note - first 3 measurements used as equilibration time, and not included in average</t>
-  </si>
-  <si>
     <t>Machine - AccuFit 9000 (Levitt Safety)</t>
   </si>
   <si>
     <t xml:space="preserve">Filtration Factor Testing.  60mL (BD Luer Lock) syringe, occluded on one end.  Filter material tightly taped over open end with packing tape.  Sampling line inserted through hole in sidewall of syringe </t>
   </si>
   <si>
-    <t>HV MERV 14</t>
-  </si>
-  <si>
     <t>Camfil Vacuum Filter MERV15 1 ply</t>
   </si>
   <si>
     <t>Camfil Vacuum Filter MERV15 2 ply</t>
   </si>
   <si>
-    <t>FILTER</t>
-  </si>
-  <si>
-    <t>Run 1</t>
-  </si>
-  <si>
-    <t>Run 2</t>
-  </si>
-  <si>
-    <t>Run 3</t>
-  </si>
-  <si>
-    <t>Run 4</t>
-  </si>
-  <si>
-    <t>Run 5</t>
-  </si>
-  <si>
-    <t>Run 6</t>
-  </si>
-  <si>
-    <t>Run 7</t>
-  </si>
-  <si>
     <t>Location:</t>
   </si>
   <si>
@@ -127,6 +97,27 @@
   </si>
   <si>
     <t>WN</t>
+  </si>
+  <si>
+    <t>Overall Filtration Factor is given by a formula, where n= no. of runs, here n=7:</t>
+  </si>
+  <si>
+    <t>Overall FF = 1/(1/ff1 + 1/ff2 + 1/ff3 + 1/ff4 + 1/ff5 + 1/ff6 +1/ff7)</t>
+  </si>
+  <si>
+    <t>Note 2</t>
+  </si>
+  <si>
+    <t>Note 1 - first 3 measurements used as equilibration time, and not included in average</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Filtration Factor (Outside particulate concentration : Inside particulate concentration, averaged by integral/time)</t>
+  </si>
+  <si>
+    <t>HV MERV 14 1 ply</t>
   </si>
 </sst>
 </file>
@@ -150,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +163,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -212,6 +209,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +579,7 @@
   <dimension ref="A1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,12 +591,12 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -608,35 +609,51 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
-      </c>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
         <v>3</v>
@@ -660,15 +677,15 @@
         <v>9</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="M7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
+      <c r="A8" s="1">
+        <v>1</v>
       </c>
       <c r="B8" s="1">
         <v>143</v>
@@ -708,8 +725,8 @@
       </c>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
+      <c r="A9" s="1">
+        <v>2</v>
       </c>
       <c r="B9" s="1">
         <v>171</v>
@@ -749,8 +766,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
+      <c r="A10" s="1">
+        <v>3</v>
       </c>
       <c r="B10" s="1">
         <v>151</v>
@@ -790,8 +807,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>23</v>
+      <c r="A11">
+        <v>4</v>
       </c>
       <c r="B11" s="3">
         <v>165</v>
@@ -831,8 +848,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>24</v>
+      <c r="A12">
+        <v>5</v>
       </c>
       <c r="B12" s="3">
         <v>165</v>
@@ -872,8 +889,8 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>25</v>
+      <c r="A13">
+        <v>6</v>
       </c>
       <c r="B13" s="3">
         <v>167</v>
@@ -913,8 +930,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
+      <c r="A14">
+        <v>7</v>
       </c>
       <c r="B14" s="3">
         <v>155</v>
@@ -954,37 +971,40 @@
       </c>
     </row>
     <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="9">
         <v>155</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="9">
         <v>53.54</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="9">
         <v>557.80999999999995</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="9">
         <v>113.09</v>
       </c>
-      <c r="G15" s="1">
+      <c r="F15" s="9">
+        <v>27.41</v>
+      </c>
+      <c r="G15" s="9">
         <v>14.56</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="9">
         <v>2366.19</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="9">
         <v>39.85</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="9">
         <v>473.91</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="9">
         <v>41.05</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="9">
         <v>107.54</v>
       </c>
     </row>
@@ -1044,7 +1064,20 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -1084,6 +1117,9 @@
       <c r="I35" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:M6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>